<commit_message>
[Vedhashni] Added the file with refactored code for signup and added validation
</commit_message>
<xml_diff>
--- a/DataDrivenForFB/Data/Data.xlsx
+++ b/DataDrivenForFB/Data/Data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F4298E-0D9A-43B5-BAAD-C56EC8E06878}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE70CB1-502D-4E19-B8D6-FD1825AEBAAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Velskar@1</t>
+  </si>
+  <si>
+    <t>karthiga</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,9 +387,18 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9843801062</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4D8DE57C-E7C9-4947-BFA7-C8856787A64B}"/>
+    <hyperlink ref="B3" r:id="rId2" display="vedha@1" xr:uid="{6C30D176-D39F-4AEE-9A4D-113D33644E37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>